<commit_message>
Updated "Release To Location" in the Release IEPD with the same structure as "Arrest Location" in the Booking IEPD.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Release_Reporting/artifacts/service_model/information_model/IEPD/documentation/CustodyRelease.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Release_Reporting/artifacts/service_model/information_model/IEPD/documentation/CustodyRelease.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="2740" windowWidth="29560" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="4820" yWindow="1340" windowWidth="29560" windowHeight="16680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CustodyStatusChangeReport" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="120">
   <si>
     <t>Race</t>
   </si>
@@ -162,19 +162,7 @@
     <t>Release To Location</t>
   </si>
   <si>
-    <t>Street Full Text</t>
-  </si>
-  <si>
     <t>Apt/Suite</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip Code</t>
   </si>
   <si>
     <t>/crr-doc:CustodyReleaseReport/nc:DocumentCreationDate/nc:DateTime</t>
@@ -334,18 +322,12 @@
     <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ActivityReasonText</t>
   </si>
   <si>
-    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationStreet/nc:StreetFullText</t>
-  </si>
-  <si>
     <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:AddressSecondaryUnitText</t>
   </si>
   <si>
     <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationCityName</t>
   </si>
   <si>
-    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/j:LocationStateNCICLISCode</t>
-  </si>
-  <si>
     <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationPostalCode</t>
   </si>
   <si>
@@ -392,6 +374,30 @@
   </si>
   <si>
     <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleasePerson/@structures:ref]/nc:PersonPhysicalFeature/nc:PhysicalFeatureDescriptionText</t>
+  </si>
+  <si>
+    <t>Street Number</t>
+  </si>
+  <si>
+    <t>Street Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> City</t>
+  </si>
+  <si>
+    <t>State Code</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationStreet/nc:StreetNumberText</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationStreet/nc:StreetName</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationStateUSPostalServiceCode</t>
   </si>
 </sst>
 </file>
@@ -557,7 +563,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="758">
+  <cellStyleXfs count="768">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1316,8 +1322,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1424,8 +1440,14 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="735" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="758">
+  <cellStyles count="768">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1804,6 +1826,11 @@
     <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2182,6 +2209,11 @@
     <cellStyle name="Hyperlink" xfId="752" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="754" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="766" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="735" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2512,11 +2544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M376"/>
+  <dimension ref="A1:M377"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14:B19"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2531,7 +2563,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="27" customFormat="1">
       <c r="A1" s="35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="28"/>
@@ -2557,7 +2589,7 @@
     </row>
     <row r="3" spans="1:13" s="9" customFormat="1" ht="14">
       <c r="A3" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2574,7 +2606,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="9" customFormat="1" ht="14">
@@ -2587,7 +2619,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="9" customFormat="1" ht="14">
@@ -2607,7 +2639,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="9" customFormat="1" ht="14">
@@ -2618,7 +2650,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="9" customFormat="1" ht="14">
@@ -2638,7 +2670,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="9" customFormat="1" ht="14">
@@ -2649,7 +2681,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="9" customFormat="1" ht="14">
@@ -2664,23 +2696,23 @@
     <row r="13" spans="1:13" s="25" customFormat="1" ht="30">
       <c r="A13" s="23"/>
       <c r="B13" s="24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
       <c r="E13" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A14" s="23"/>
       <c r="B14" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="29"/>
       <c r="E14" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="31"/>
@@ -2694,12 +2726,12 @@
     <row r="15" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A15" s="23"/>
       <c r="B15" s="24" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="29"/>
       <c r="E15" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F15" s="30"/>
       <c r="G15" s="31"/>
@@ -2713,12 +2745,12 @@
     <row r="16" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A16" s="23"/>
       <c r="B16" s="24" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="29"/>
       <c r="E16" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F16" s="30"/>
       <c r="G16" s="31"/>
@@ -2732,12 +2764,12 @@
     <row r="17" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A17" s="23"/>
       <c r="B17" s="24" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="29"/>
       <c r="E17" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="31"/>
@@ -2751,12 +2783,12 @@
     <row r="18" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A18" s="23"/>
       <c r="B18" s="24" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="29"/>
       <c r="E18" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="31"/>
@@ -2770,12 +2802,12 @@
     <row r="19" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A19" s="23"/>
       <c r="B19" s="24" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="29"/>
       <c r="E19" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>
@@ -2796,7 +2828,7 @@
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2809,7 +2841,7 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2822,7 +2854,7 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2835,7 +2867,7 @@
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="9" customFormat="1" ht="42">
@@ -2848,7 +2880,7 @@
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="9" customFormat="1" ht="42">
@@ -2861,7 +2893,7 @@
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="9" customFormat="1" ht="42">
@@ -2874,7 +2906,7 @@
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2887,7 +2919,7 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2900,7 +2932,7 @@
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2913,7 +2945,7 @@
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2926,7 +2958,7 @@
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2939,7 +2971,7 @@
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2950,12 +2982,12 @@
       <c r="C32" s="8"/>
       <c r="D32" s="7"/>
       <c r="E32" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="22" customFormat="1">
       <c r="A33" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -2972,7 +3004,7 @@
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="26" customFormat="1" ht="60">
@@ -2985,7 +3017,7 @@
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="26" customFormat="1" ht="60">
@@ -2998,7 +3030,7 @@
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="26" customFormat="1" ht="60">
@@ -3011,7 +3043,7 @@
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="26" customFormat="1" ht="45">
@@ -3024,12 +3056,12 @@
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="14" customFormat="1">
       <c r="A39" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -3038,27 +3070,27 @@
     </row>
     <row r="40" spans="1:5" s="32" customFormat="1" ht="28">
       <c r="B40" s="33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1">
       <c r="A41" s="16"/>
       <c r="B41" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" ht="30">
@@ -3071,12 +3103,12 @@
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="19" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1">
       <c r="A43" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -3085,15 +3117,15 @@
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" ht="14">
       <c r="B44" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1">
       <c r="A45" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -3102,10 +3134,10 @@
     </row>
     <row r="46" spans="1:5" s="10" customFormat="1" ht="14">
       <c r="B46" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="10" customFormat="1" ht="28">
@@ -3117,7 +3149,7 @@
         <v>43</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="9" customFormat="1" ht="14">
@@ -3128,7 +3160,7 @@
         <v>45</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="9" customFormat="1" ht="14">
@@ -3140,84 +3172,102 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" s="9" customFormat="1" ht="28">
-      <c r="B50" s="8" t="s">
+    <row r="50" spans="1:5" s="37" customFormat="1" ht="30">
+      <c r="A50" s="25"/>
+      <c r="B50" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="37" customFormat="1" ht="30">
+      <c r="A51" s="25"/>
+      <c r="B51" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="37" customFormat="1" ht="30">
+      <c r="A52" s="25"/>
+      <c r="B52" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="37" customFormat="1" ht="30">
+      <c r="A53" s="25"/>
+      <c r="B53" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="37" customFormat="1" ht="30">
+      <c r="A54" s="25"/>
+      <c r="B54" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="37" customFormat="1" ht="30">
+      <c r="A55" s="25"/>
+      <c r="B55" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="22" customFormat="1">
+      <c r="A56" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+    </row>
+    <row r="57" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B57" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="26" customFormat="1">
+      <c r="B58" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58" s="17" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="B51" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A52" s="6"/>
-      <c r="B52" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="9" customFormat="1" ht="28">
-      <c r="B53" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="9" customFormat="1" ht="28">
-      <c r="B54" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="22" customFormat="1">
-      <c r="A55" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-    </row>
-    <row r="56" spans="1:5" s="26" customFormat="1" ht="30">
-      <c r="B56" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E56" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="26" customFormat="1">
-      <c r="B57" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E57" s="17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="9" customFormat="1" ht="14"/>
     <row r="59" spans="1:5" s="9" customFormat="1" ht="14"/>
     <row r="60" spans="1:5" s="9" customFormat="1" ht="14"/>
     <row r="61" spans="1:5" s="9" customFormat="1" ht="14"/>
     <row r="62" spans="1:5" s="9" customFormat="1" ht="14"/>
-    <row r="63" spans="1:5">
-      <c r="A63" s="34"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-    </row>
+    <row r="63" spans="1:5" s="9" customFormat="1" ht="14"/>
     <row r="64" spans="1:5">
       <c r="A64" s="34"/>
       <c r="B64" s="34"/>
@@ -5408,6 +5458,13 @@
       <c r="C376" s="34"/>
       <c r="D376" s="34"/>
       <c r="E376" s="34"/>
+    </row>
+    <row r="377" spans="1:5">
+      <c r="A377" s="34"/>
+      <c r="B377" s="34"/>
+      <c r="C377" s="34"/>
+      <c r="D377" s="34"/>
+      <c r="E377" s="34"/>
     </row>
   </sheetData>
   <sortState ref="A8:J35">

</xml_diff>

<commit_message>
Added the Person_Health_Information_Search_Results to the IEPDs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Release_Reporting/artifacts/service_model/information_model/IEPD/documentation/CustodyRelease.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Release_Reporting/artifacts/service_model/information_model/IEPD/documentation/CustodyRelease.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="1340" windowWidth="29560" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="5260" yWindow="1660" windowWidth="29560" windowHeight="16680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CustodyStatusChangeReport" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="159">
   <si>
     <t>Race</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>Behavioral Health</t>
-  </si>
-  <si>
-    <t>Diagnosis</t>
   </si>
   <si>
     <t>SMI Indicator</t>
@@ -331,12 +328,6 @@
     <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationPostalCode</t>
   </si>
   <si>
-    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation/j:Evaluation/j:EvaluationDiagnosisDescriptionText</t>
-  </si>
-  <si>
-    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation/crr-ext:SeriousMentalIllnessIndicator</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -398,6 +389,132 @@
   </si>
   <si>
     <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Release/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationStateUSPostalServiceCode</t>
+  </si>
+  <si>
+    <t>Serious Mental Ilness</t>
+  </si>
+  <si>
+    <t>HRN Indicator</t>
+  </si>
+  <si>
+    <t>High Risk Needs</t>
+  </si>
+  <si>
+    <t>SA Indicator</t>
+  </si>
+  <si>
+    <t>Substance Abuse</t>
+  </si>
+  <si>
+    <t>GMHC Indicatior</t>
+  </si>
+  <si>
+    <t>General Mental Health Condition</t>
+  </si>
+  <si>
+    <t>Diagnosis Description</t>
+  </si>
+  <si>
+    <t>Treatment Start Date</t>
+  </si>
+  <si>
+    <t>Treatment End Date</t>
+  </si>
+  <si>
+    <t>Treatment Provider</t>
+  </si>
+  <si>
+    <t>TCO Indicator</t>
+  </si>
+  <si>
+    <t>Treeatment Court Ordered</t>
+  </si>
+  <si>
+    <t>TA Indicator</t>
+  </si>
+  <si>
+    <t>Treatment Active Indicator</t>
+  </si>
+  <si>
+    <t>Prescribed Medication Name</t>
+  </si>
+  <si>
+    <t>Medication Product ID</t>
+  </si>
+  <si>
+    <t>Medication Dispensing Date</t>
+  </si>
+  <si>
+    <t>Medication Dose Text</t>
+  </si>
+  <si>
+    <t>Medicaid Indicator</t>
+  </si>
+  <si>
+    <t>Regional Behavioral Health Authority Assigment Text</t>
+  </si>
+  <si>
+    <t>Care Episode</t>
+  </si>
+  <si>
+    <t>Care EpisodeStart Date</t>
+  </si>
+  <si>
+    <t>Care Episode End Date</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/crr-ext:SeriousMentalIllnessIndicator</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/crr-ext:HighRiskNeedsIndicator</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/crr-ext:SubstanceAbuseIndicator</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/crr-ext:GeneralMentalHealthConditionIndicator</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/j:Evaluation/j:EvaluationDiagnosisDescriptionText</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/nc:ActivityDateRange/nc:StartDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/nc:ActivityDateRange/nc:EndDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/nc:TreatmentProvider/nc:EntityOrganization/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/crr-ext:TreatmentCourtOrderedIndicator</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/crr-ext:TreatmentActiveIndicator</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/crr-ext:PrescribedMedication/cyfs:Medication/nc:ItemName</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/crr-ext:PrescribedMedication/cyfs:Medication/crr-ext:MedicationGeneralProductIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/crr-ext:PrescribedMedication/cyfs:MedicationDispensingDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/crr-ext:PrescribedMedication/cyfs:MedicationDoseMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/hs:MedicaidIndicator</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonBehavioralHealthInformation/@structures:ref]/crr-ext:RegionalBehavioralHealthAuthorityAssignmentText</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:CareEpisode[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonCareEpisode/@structures:ref]/nc:ActivityDateRange/nc:StartDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:CareEpisode[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person/crr-ext:PersonCareEpisode/@structures:ref]/nc:ActivityDateRange/nc:EndDate/nc:Date</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1450,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1437,13 +1554,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="735" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="735" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2544,11 +2667,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M377"/>
+  <dimension ref="A1:M394"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="2" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2562,10 +2685,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="27" customFormat="1">
-      <c r="A1" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="35"/>
+      <c r="A1" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="37"/>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
@@ -2701,18 +2824,18 @@
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
       <c r="E13" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A14" s="23"/>
       <c r="B14" s="24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="29"/>
       <c r="E14" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="31"/>
@@ -2726,12 +2849,12 @@
     <row r="15" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A15" s="23"/>
       <c r="B15" s="24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="29"/>
       <c r="E15" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F15" s="30"/>
       <c r="G15" s="31"/>
@@ -2745,12 +2868,12 @@
     <row r="16" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A16" s="23"/>
       <c r="B16" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="29"/>
       <c r="E16" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F16" s="30"/>
       <c r="G16" s="31"/>
@@ -2764,12 +2887,12 @@
     <row r="17" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A17" s="23"/>
       <c r="B17" s="24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="29"/>
       <c r="E17" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="31"/>
@@ -2783,12 +2906,12 @@
     <row r="18" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A18" s="23"/>
       <c r="B18" s="24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="29"/>
       <c r="E18" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="31"/>
@@ -2802,12 +2925,12 @@
     <row r="19" spans="1:13" s="25" customFormat="1" ht="28">
       <c r="A19" s="23"/>
       <c r="B19" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="29"/>
       <c r="E19" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>
@@ -2828,7 +2951,7 @@
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2841,7 +2964,7 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2854,7 +2977,7 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2867,7 +2990,7 @@
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="9" customFormat="1" ht="42">
@@ -2880,7 +3003,7 @@
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="9" customFormat="1" ht="42">
@@ -2893,7 +3016,7 @@
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="9" customFormat="1" ht="42">
@@ -2906,7 +3029,7 @@
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2919,7 +3042,7 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2932,7 +3055,7 @@
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2945,7 +3068,7 @@
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2958,7 +3081,7 @@
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2971,7 +3094,7 @@
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="9" customFormat="1" ht="28">
@@ -2982,7 +3105,7 @@
       <c r="C32" s="8"/>
       <c r="D32" s="7"/>
       <c r="E32" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="22" customFormat="1">
@@ -3004,7 +3127,7 @@
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="26" customFormat="1" ht="60">
@@ -3017,7 +3140,7 @@
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="26" customFormat="1" ht="60">
@@ -3030,7 +3153,7 @@
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="26" customFormat="1" ht="60">
@@ -3043,7 +3166,7 @@
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="26" customFormat="1" ht="45">
@@ -3056,7 +3179,7 @@
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="14" customFormat="1">
@@ -3077,7 +3200,7 @@
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1">
@@ -3090,7 +3213,7 @@
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" ht="30">
@@ -3103,12 +3226,12 @@
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1">
       <c r="A43" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -3117,15 +3240,15 @@
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" ht="14">
       <c r="B44" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1">
       <c r="A45" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -3134,10 +3257,10 @@
     </row>
     <row r="46" spans="1:5" s="10" customFormat="1" ht="14">
       <c r="B46" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="10" customFormat="1" ht="28">
@@ -3149,7 +3272,7 @@
         <v>43</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="9" customFormat="1" ht="14">
@@ -3160,7 +3283,7 @@
         <v>45</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="9" customFormat="1" ht="14">
@@ -3172,221 +3295,257 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" s="37" customFormat="1" ht="30">
+    <row r="50" spans="1:5" s="36" customFormat="1" ht="30">
       <c r="A50" s="25"/>
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="35" t="s">
         <v>47</v>
       </c>
       <c r="C50" s="25"/>
       <c r="D50" s="25"/>
       <c r="E50" s="24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="37" customFormat="1" ht="30">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="36" customFormat="1" ht="30">
       <c r="A51" s="25"/>
-      <c r="B51" s="36" t="s">
-        <v>112</v>
+      <c r="B51" s="35" t="s">
+        <v>109</v>
       </c>
       <c r="C51" s="25"/>
       <c r="D51" s="25"/>
       <c r="E51" s="24" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="37" customFormat="1" ht="30">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="36" customFormat="1" ht="30">
       <c r="A52" s="25"/>
-      <c r="B52" s="36" t="s">
-        <v>113</v>
+      <c r="B52" s="35" t="s">
+        <v>110</v>
       </c>
       <c r="C52" s="25"/>
       <c r="D52" s="25"/>
       <c r="E52" s="24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="37" customFormat="1" ht="30">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="36" customFormat="1" ht="30">
       <c r="A53" s="25"/>
-      <c r="B53" s="36" t="s">
-        <v>114</v>
+      <c r="B53" s="35" t="s">
+        <v>111</v>
       </c>
       <c r="C53" s="25"/>
       <c r="D53" s="25"/>
       <c r="E53" s="24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="37" customFormat="1" ht="30">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="36" customFormat="1" ht="30">
       <c r="A54" s="25"/>
-      <c r="B54" s="36" t="s">
-        <v>115</v>
+      <c r="B54" s="35" t="s">
+        <v>112</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
       <c r="E54" s="24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="37" customFormat="1" ht="30">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="36" customFormat="1" ht="30">
       <c r="A55" s="25"/>
-      <c r="B55" s="36" t="s">
-        <v>116</v>
+      <c r="B55" s="35" t="s">
+        <v>113</v>
       </c>
       <c r="C55" s="25"/>
       <c r="D55" s="25"/>
       <c r="E55" s="24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="22" customFormat="1">
-      <c r="A56" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="26" customFormat="1">
+      <c r="A56" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-    </row>
-    <row r="57" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+    </row>
+    <row r="57" spans="1:5" s="26" customFormat="1" ht="45">
       <c r="B57" s="26" t="s">
         <v>62</v>
       </c>
+      <c r="C57" s="26" t="s">
+        <v>117</v>
+      </c>
       <c r="E57" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="26" customFormat="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="26" customFormat="1" ht="30">
       <c r="B58" s="24" t="s">
-        <v>63</v>
+        <v>118</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>119</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="9" customFormat="1" ht="14"/>
-    <row r="60" spans="1:5" s="9" customFormat="1" ht="14"/>
-    <row r="61" spans="1:5" s="9" customFormat="1" ht="14"/>
-    <row r="62" spans="1:5" s="9" customFormat="1" ht="14"/>
-    <row r="63" spans="1:5" s="9" customFormat="1" ht="14"/>
-    <row r="64" spans="1:5">
-      <c r="A64" s="34"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="34"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="34"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="34"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="34"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="34"/>
-      <c r="B68" s="34"/>
-      <c r="C68" s="34"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="34"/>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="34"/>
-      <c r="B69" s="34"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="34"/>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="34"/>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="34"/>
-      <c r="B71" s="34"/>
-      <c r="C71" s="34"/>
-      <c r="D71" s="34"/>
-      <c r="E71" s="34"/>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="34"/>
-      <c r="B72" s="34"/>
-      <c r="C72" s="34"/>
-      <c r="D72" s="34"/>
-      <c r="E72" s="34"/>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="34"/>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="34"/>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="34"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="34"/>
-      <c r="B76" s="34"/>
-      <c r="C76" s="34"/>
-      <c r="D76" s="34"/>
-      <c r="E76" s="34"/>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="34"/>
-      <c r="B77" s="34"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="34"/>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="34"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="34"/>
-      <c r="D78" s="34"/>
-      <c r="E78" s="34"/>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="34"/>
-      <c r="B79" s="34"/>
-      <c r="C79" s="34"/>
-      <c r="D79" s="34"/>
-      <c r="E79" s="34"/>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="34"/>
-      <c r="B80" s="34"/>
-      <c r="C80" s="34"/>
-      <c r="D80" s="34"/>
-      <c r="E80" s="34"/>
-    </row>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B59" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="26" customFormat="1" ht="45">
+      <c r="B60" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B61" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B62" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B63" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="26" customFormat="1" ht="60">
+      <c r="B64" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B65" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B66" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B67" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="26" customFormat="1" ht="45">
+      <c r="B68" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="26" customFormat="1" ht="45">
+      <c r="B69" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="26" customFormat="1" ht="45">
+      <c r="B70" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B71" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="26" customFormat="1" ht="45">
+      <c r="B72" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="26" customFormat="1">
+      <c r="A73" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B73" s="39"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+    </row>
+    <row r="74" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B74" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="26" customFormat="1" ht="30">
+      <c r="B75" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="9" customFormat="1" ht="14"/>
+    <row r="77" spans="1:5" s="9" customFormat="1" ht="14"/>
+    <row r="78" spans="1:5" s="9" customFormat="1" ht="14"/>
+    <row r="79" spans="1:5" s="9" customFormat="1" ht="14"/>
+    <row r="80" spans="1:5" s="9" customFormat="1" ht="14"/>
     <row r="81" spans="1:5">
       <c r="A81" s="34"/>
       <c r="B81" s="34"/>
@@ -5465,6 +5624,125 @@
       <c r="C377" s="34"/>
       <c r="D377" s="34"/>
       <c r="E377" s="34"/>
+    </row>
+    <row r="378" spans="1:5">
+      <c r="A378" s="34"/>
+      <c r="B378" s="34"/>
+      <c r="C378" s="34"/>
+      <c r="D378" s="34"/>
+      <c r="E378" s="34"/>
+    </row>
+    <row r="379" spans="1:5">
+      <c r="A379" s="34"/>
+      <c r="B379" s="34"/>
+      <c r="C379" s="34"/>
+      <c r="D379" s="34"/>
+      <c r="E379" s="34"/>
+    </row>
+    <row r="380" spans="1:5">
+      <c r="A380" s="34"/>
+      <c r="B380" s="34"/>
+      <c r="C380" s="34"/>
+      <c r="D380" s="34"/>
+      <c r="E380" s="34"/>
+    </row>
+    <row r="381" spans="1:5">
+      <c r="A381" s="34"/>
+      <c r="B381" s="34"/>
+      <c r="C381" s="34"/>
+      <c r="D381" s="34"/>
+      <c r="E381" s="34"/>
+    </row>
+    <row r="382" spans="1:5">
+      <c r="A382" s="34"/>
+      <c r="B382" s="34"/>
+      <c r="C382" s="34"/>
+      <c r="D382" s="34"/>
+      <c r="E382" s="34"/>
+    </row>
+    <row r="383" spans="1:5">
+      <c r="A383" s="34"/>
+      <c r="B383" s="34"/>
+      <c r="C383" s="34"/>
+      <c r="D383" s="34"/>
+      <c r="E383" s="34"/>
+    </row>
+    <row r="384" spans="1:5">
+      <c r="A384" s="34"/>
+      <c r="B384" s="34"/>
+      <c r="C384" s="34"/>
+      <c r="D384" s="34"/>
+      <c r="E384" s="34"/>
+    </row>
+    <row r="385" spans="1:5">
+      <c r="A385" s="34"/>
+      <c r="B385" s="34"/>
+      <c r="C385" s="34"/>
+      <c r="D385" s="34"/>
+      <c r="E385" s="34"/>
+    </row>
+    <row r="386" spans="1:5">
+      <c r="A386" s="34"/>
+      <c r="B386" s="34"/>
+      <c r="C386" s="34"/>
+      <c r="D386" s="34"/>
+      <c r="E386" s="34"/>
+    </row>
+    <row r="387" spans="1:5">
+      <c r="A387" s="34"/>
+      <c r="B387" s="34"/>
+      <c r="C387" s="34"/>
+      <c r="D387" s="34"/>
+      <c r="E387" s="34"/>
+    </row>
+    <row r="388" spans="1:5">
+      <c r="A388" s="34"/>
+      <c r="B388" s="34"/>
+      <c r="C388" s="34"/>
+      <c r="D388" s="34"/>
+      <c r="E388" s="34"/>
+    </row>
+    <row r="389" spans="1:5">
+      <c r="A389" s="34"/>
+      <c r="B389" s="34"/>
+      <c r="C389" s="34"/>
+      <c r="D389" s="34"/>
+      <c r="E389" s="34"/>
+    </row>
+    <row r="390" spans="1:5">
+      <c r="A390" s="34"/>
+      <c r="B390" s="34"/>
+      <c r="C390" s="34"/>
+      <c r="D390" s="34"/>
+      <c r="E390" s="34"/>
+    </row>
+    <row r="391" spans="1:5">
+      <c r="A391" s="34"/>
+      <c r="B391" s="34"/>
+      <c r="C391" s="34"/>
+      <c r="D391" s="34"/>
+      <c r="E391" s="34"/>
+    </row>
+    <row r="392" spans="1:5">
+      <c r="A392" s="34"/>
+      <c r="B392" s="34"/>
+      <c r="C392" s="34"/>
+      <c r="D392" s="34"/>
+      <c r="E392" s="34"/>
+    </row>
+    <row r="393" spans="1:5">
+      <c r="A393" s="34"/>
+      <c r="B393" s="34"/>
+      <c r="C393" s="34"/>
+      <c r="D393" s="34"/>
+      <c r="E393" s="34"/>
+    </row>
+    <row r="394" spans="1:5">
+      <c r="A394" s="34"/>
+      <c r="B394" s="34"/>
+      <c r="C394" s="34"/>
+      <c r="D394" s="34"/>
+      <c r="E394" s="34"/>
     </row>
   </sheetData>
   <sortState ref="A8:J35">

</xml_diff>